<commit_message>
update with discovery patterns
</commit_message>
<xml_diff>
--- a/predictions/CUIS_for_overlap.xlsx
+++ b/predictions/CUIS_for_overlap.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schut184/Desktop/covid_discovery/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E13CFA-8107-CF45-ABD6-A7365B302878}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E1BB33-AC49-1141-9B79-DC19F278CF9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14340" yWindow="1880" windowWidth="14080" windowHeight="15560" xr2:uid="{1E2092A4-91F0-B943-9E38-B5A621C7573B}"/>
+    <workbookView xWindow="11880" yWindow="500" windowWidth="16540" windowHeight="16940" xr2:uid="{1E2092A4-91F0-B943-9E38-B5A621C7573B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="391">
   <si>
     <t>STELP</t>
   </si>
@@ -1138,6 +1138,75 @@
   </si>
   <si>
     <t>C0037663</t>
+  </si>
+  <si>
+    <t>Discovery Patterns</t>
+  </si>
+  <si>
+    <t>C0025853</t>
+  </si>
+  <si>
+    <t>C0077144</t>
+  </si>
+  <si>
+    <t>C0056855</t>
+  </si>
+  <si>
+    <t>C2347168</t>
+  </si>
+  <si>
+    <t>C1373111</t>
+  </si>
+  <si>
+    <t>C0025865</t>
+  </si>
+  <si>
+    <t>C0252643</t>
+  </si>
+  <si>
+    <t>C0016410</t>
+  </si>
+  <si>
+    <t>C0014921</t>
+  </si>
+  <si>
+    <t>C0529793</t>
+  </si>
+  <si>
+    <t>C0016860</t>
+  </si>
+  <si>
+    <t>C0004905</t>
+  </si>
+  <si>
+    <t>C1121991</t>
+  </si>
+  <si>
+    <t>C0062022</t>
+  </si>
+  <si>
+    <t>C1443650</t>
+  </si>
+  <si>
+    <t>C1520059</t>
+  </si>
+  <si>
+    <t>C2746052</t>
+  </si>
+  <si>
+    <t>C1268567</t>
+  </si>
+  <si>
+    <t>C0055895</t>
+  </si>
+  <si>
+    <t>C0066700</t>
+  </si>
+  <si>
+    <t>C3537128</t>
+  </si>
+  <si>
+    <t>C0599685</t>
   </si>
 </sst>
 </file>
@@ -1498,10 +1567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFA8EB9-B48F-CC45-98CC-F1A82873E357}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1509,9 +1578,10 @@
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1539,16 +1609,19 @@
       <c r="I1" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>163</v>
+      <c r="C2" s="1" t="s">
+        <v>369</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -1568,16 +1641,19 @@
       <c r="I2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>322</v>
+      <c r="C3" s="1" t="s">
+        <v>370</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -1597,16 +1673,19 @@
       <c r="I3" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
-        <v>323</v>
+      <c r="C4" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -1626,16 +1705,19 @@
       <c r="I4" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>324</v>
+      <c r="C5" s="1" t="s">
+        <v>371</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -1655,16 +1737,19 @@
       <c r="I5" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
-        <v>325</v>
+      <c r="C6" s="1" t="s">
+        <v>372</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>
@@ -1684,16 +1769,19 @@
       <c r="I6" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
-        <v>326</v>
+      <c r="C7" s="1" t="s">
+        <v>373</v>
       </c>
       <c r="D7" t="s">
         <v>30</v>
@@ -1713,16 +1801,19 @@
       <c r="I7" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
-        <v>263</v>
+      <c r="C8" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="D8" t="s">
         <v>35</v>
@@ -1742,16 +1833,19 @@
       <c r="I8" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
-        <v>274</v>
+      <c r="C9" s="1" t="s">
+        <v>374</v>
       </c>
       <c r="D9" t="s">
         <v>40</v>
@@ -1771,16 +1865,19 @@
       <c r="I9" s="2" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>43</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
       </c>
-      <c r="C10" t="s">
-        <v>327</v>
+      <c r="C10" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="D10" t="s">
         <v>45</v>
@@ -1800,16 +1897,19 @@
       <c r="I10" s="2" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>48</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
       </c>
-      <c r="C11" t="s">
-        <v>328</v>
+      <c r="C11" s="1" t="s">
+        <v>375</v>
       </c>
       <c r="D11" t="s">
         <v>50</v>
@@ -1829,16 +1929,19 @@
       <c r="I11" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>53</v>
       </c>
-      <c r="C12" t="s">
-        <v>329</v>
+      <c r="C12" s="1" t="s">
+        <v>376</v>
       </c>
       <c r="D12" t="s">
         <v>54</v>
@@ -1858,16 +1961,19 @@
       <c r="I12" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>57</v>
       </c>
       <c r="B13" t="s">
         <v>58</v>
       </c>
-      <c r="C13" t="s">
-        <v>330</v>
+      <c r="C13" s="1" t="s">
+        <v>377</v>
       </c>
       <c r="D13" t="s">
         <v>59</v>
@@ -1887,16 +1993,19 @@
       <c r="I13" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>62</v>
       </c>
       <c r="B14" t="s">
         <v>63</v>
       </c>
-      <c r="C14" t="s">
-        <v>331</v>
+      <c r="C14" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="D14" t="s">
         <v>64</v>
@@ -1916,16 +2025,19 @@
       <c r="I14" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>67</v>
       </c>
       <c r="B15" t="s">
         <v>68</v>
       </c>
-      <c r="C15" t="s">
-        <v>270</v>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="D15" t="s">
         <v>69</v>
@@ -1945,16 +2057,19 @@
       <c r="I15" s="2" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>72</v>
       </c>
       <c r="B16" t="s">
         <v>73</v>
       </c>
-      <c r="C16" t="s">
-        <v>332</v>
+      <c r="C16" s="1" t="s">
+        <v>378</v>
       </c>
       <c r="D16" t="s">
         <v>74</v>
@@ -1974,16 +2089,19 @@
       <c r="I16" s="2" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>77</v>
       </c>
       <c r="B17" t="s">
         <v>78</v>
       </c>
-      <c r="C17" t="s">
-        <v>333</v>
+      <c r="C17" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="D17" t="s">
         <v>79</v>
@@ -2003,16 +2121,19 @@
       <c r="I17" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>82</v>
       </c>
       <c r="B18" t="s">
         <v>83</v>
       </c>
-      <c r="C18" t="s">
-        <v>334</v>
+      <c r="C18" s="1" t="s">
+        <v>379</v>
       </c>
       <c r="D18" t="s">
         <v>84</v>
@@ -2029,16 +2150,19 @@
       <c r="I18" s="2" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
       <c r="B19" t="s">
         <v>87</v>
       </c>
-      <c r="C19" t="s">
-        <v>335</v>
+      <c r="C19" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="D19" t="s">
         <v>88</v>
@@ -2055,16 +2179,19 @@
       <c r="I19" s="2" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>91</v>
       </c>
       <c r="B20" t="s">
         <v>92</v>
       </c>
-      <c r="C20" t="s">
-        <v>336</v>
+      <c r="C20" s="1" t="s">
+        <v>380</v>
       </c>
       <c r="D20" t="s">
         <v>93</v>
@@ -2081,16 +2208,19 @@
       <c r="I20" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>14</v>
       </c>
       <c r="B21" t="s">
         <v>96</v>
       </c>
-      <c r="C21" t="s">
-        <v>337</v>
+      <c r="C21" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D21" t="s">
         <v>97</v>
@@ -2107,16 +2237,19 @@
       <c r="I21" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>100</v>
       </c>
       <c r="B22" t="s">
         <v>101</v>
       </c>
-      <c r="C22" t="s">
-        <v>338</v>
+      <c r="C22" s="1" t="s">
+        <v>381</v>
       </c>
       <c r="D22" t="s">
         <v>102</v>
@@ -2133,16 +2266,19 @@
       <c r="I22" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>105</v>
       </c>
       <c r="B23" t="s">
         <v>106</v>
       </c>
-      <c r="C23" t="s">
-        <v>339</v>
+      <c r="C23" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="D23" t="s">
         <v>107</v>
@@ -2159,16 +2295,19 @@
       <c r="I23" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>14</v>
       </c>
       <c r="B24" t="s">
         <v>110</v>
       </c>
-      <c r="C24" t="s">
-        <v>340</v>
+      <c r="C24" s="1" t="s">
+        <v>382</v>
       </c>
       <c r="D24" t="s">
         <v>111</v>
@@ -2185,16 +2324,19 @@
       <c r="I24" s="2" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>114</v>
       </c>
       <c r="B25" t="s">
         <v>115</v>
       </c>
-      <c r="C25" t="s">
-        <v>341</v>
+      <c r="C25" s="1" t="s">
+        <v>383</v>
       </c>
       <c r="D25" t="s">
         <v>116</v>
@@ -2211,16 +2353,19 @@
       <c r="I25" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
       <c r="B26" t="s">
         <v>119</v>
       </c>
-      <c r="C26" t="s">
-        <v>342</v>
+      <c r="C26" s="1" t="s">
+        <v>263</v>
       </c>
       <c r="D26" t="s">
         <v>120</v>
@@ -2237,16 +2382,19 @@
       <c r="I26" s="2" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>123</v>
       </c>
       <c r="B27" t="s">
         <v>124</v>
       </c>
-      <c r="C27" t="s">
-        <v>343</v>
+      <c r="C27" s="1" t="s">
+        <v>384</v>
       </c>
       <c r="D27" t="s">
         <v>125</v>
@@ -2263,16 +2411,19 @@
       <c r="I27" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>128</v>
       </c>
       <c r="B28" t="s">
         <v>129</v>
       </c>
-      <c r="C28" t="s">
-        <v>344</v>
+      <c r="C28" s="1" t="s">
+        <v>385</v>
       </c>
       <c r="D28" t="s">
         <v>130</v>
@@ -2289,16 +2440,19 @@
       <c r="I28" s="2" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>133</v>
       </c>
       <c r="B29" t="s">
         <v>134</v>
       </c>
-      <c r="C29" t="s">
-        <v>345</v>
+      <c r="C29" s="1" t="s">
+        <v>386</v>
       </c>
       <c r="D29" t="s">
         <v>135</v>
@@ -2315,16 +2469,19 @@
       <c r="I29" s="2" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>138</v>
       </c>
       <c r="B30" t="s">
         <v>139</v>
       </c>
-      <c r="C30" t="s">
-        <v>346</v>
+      <c r="C30" s="1" t="s">
+        <v>387</v>
       </c>
       <c r="D30" t="s">
         <v>140</v>
@@ -2341,16 +2498,19 @@
       <c r="I30" s="2" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
       <c r="B31" t="s">
         <v>144</v>
       </c>
-      <c r="C31" t="s">
-        <v>347</v>
+      <c r="C31" s="1" t="s">
+        <v>388</v>
       </c>
       <c r="D31" t="s">
         <v>145</v>
@@ -2367,16 +2527,19 @@
       <c r="I31" s="2" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>105</v>
       </c>
       <c r="B32" t="s">
         <v>148</v>
       </c>
-      <c r="C32" t="s">
-        <v>348</v>
+      <c r="C32" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="D32" t="s">
         <v>149</v>
@@ -2390,16 +2553,19 @@
       <c r="H32" s="1" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J32" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>21</v>
       </c>
       <c r="B33" t="s">
         <v>152</v>
       </c>
-      <c r="C33" t="s">
-        <v>349</v>
+      <c r="C33" s="1" t="s">
+        <v>389</v>
       </c>
       <c r="D33" t="s">
         <v>153</v>
@@ -2413,16 +2579,19 @@
       <c r="H33" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J33" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>156</v>
       </c>
       <c r="B34" t="s">
         <v>157</v>
       </c>
-      <c r="C34" t="s">
-        <v>350</v>
+      <c r="C34" s="1" t="s">
+        <v>390</v>
       </c>
       <c r="D34" t="s">
         <v>158</v>
@@ -2436,17 +2605,17 @@
       <c r="H34" s="1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J34" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>161</v>
       </c>
       <c r="B35" t="s">
         <v>162</v>
       </c>
-      <c r="C35" t="s">
-        <v>351</v>
-      </c>
       <c r="D35" t="s">
         <v>163</v>
       </c>
@@ -2459,17 +2628,17 @@
       <c r="H35" s="1" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J35" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>166</v>
       </c>
       <c r="B36" t="s">
         <v>167</v>
       </c>
-      <c r="C36" t="s">
-        <v>352</v>
-      </c>
       <c r="D36" t="s">
         <v>168</v>
       </c>
@@ -2482,17 +2651,17 @@
       <c r="H36" s="1" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J36" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>171</v>
       </c>
       <c r="B37" t="s">
         <v>172</v>
       </c>
-      <c r="C37" t="s">
-        <v>353</v>
-      </c>
       <c r="D37" t="s">
         <v>173</v>
       </c>
@@ -2505,17 +2674,17 @@
       <c r="H37" s="1" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J37" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>128</v>
       </c>
       <c r="B38" t="s">
         <v>176</v>
       </c>
-      <c r="C38" t="s">
-        <v>354</v>
-      </c>
       <c r="D38" t="s">
         <v>177</v>
       </c>
@@ -2528,17 +2697,17 @@
       <c r="H38" s="1" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J38" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>180</v>
       </c>
       <c r="B39" t="s">
         <v>181</v>
       </c>
-      <c r="C39" t="s">
-        <v>355</v>
-      </c>
       <c r="D39" t="s">
         <v>182</v>
       </c>
@@ -2551,17 +2720,17 @@
       <c r="H39" s="1" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J39" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>185</v>
       </c>
       <c r="B40" t="s">
         <v>186</v>
       </c>
-      <c r="C40" t="s">
-        <v>356</v>
-      </c>
       <c r="D40" t="s">
         <v>187</v>
       </c>
@@ -2574,17 +2743,17 @@
       <c r="H40" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J40" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>190</v>
       </c>
       <c r="B41" t="s">
         <v>191</v>
       </c>
-      <c r="C41" t="s">
-        <v>357</v>
-      </c>
       <c r="D41" t="s">
         <v>192</v>
       </c>
@@ -2597,17 +2766,17 @@
       <c r="H41" s="1" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J41" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>195</v>
       </c>
       <c r="B42" t="s">
         <v>196</v>
       </c>
-      <c r="C42" t="s">
-        <v>358</v>
-      </c>
       <c r="D42" t="s">
         <v>197</v>
       </c>
@@ -2620,17 +2789,17 @@
       <c r="H42" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J42" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>16</v>
       </c>
       <c r="B43" t="s">
         <v>200</v>
       </c>
-      <c r="C43" t="s">
-        <v>359</v>
-      </c>
       <c r="D43" t="s">
         <v>201</v>
       </c>
@@ -2640,17 +2809,17 @@
       <c r="F43" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J43" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>204</v>
       </c>
       <c r="B44" t="s">
         <v>205</v>
       </c>
-      <c r="C44" t="s">
-        <v>360</v>
-      </c>
       <c r="D44" t="s">
         <v>206</v>
       </c>
@@ -2660,17 +2829,17 @@
       <c r="F44" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J44" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>209</v>
       </c>
       <c r="B45" t="s">
         <v>210</v>
       </c>
-      <c r="C45" t="s">
-        <v>361</v>
-      </c>
       <c r="D45" t="s">
         <v>211</v>
       </c>
@@ -2680,17 +2849,17 @@
       <c r="F45" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J45" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>214</v>
       </c>
       <c r="B46" t="s">
         <v>215</v>
       </c>
-      <c r="C46" t="s">
-        <v>362</v>
-      </c>
       <c r="D46" t="s">
         <v>216</v>
       </c>
@@ -2700,17 +2869,17 @@
       <c r="F46" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J46" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>219</v>
       </c>
       <c r="B47" t="s">
         <v>220</v>
       </c>
-      <c r="C47" t="s">
-        <v>363</v>
-      </c>
       <c r="D47" t="s">
         <v>221</v>
       </c>
@@ -2720,17 +2889,17 @@
       <c r="F47" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J47" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>224</v>
       </c>
       <c r="B48" t="s">
         <v>225</v>
       </c>
-      <c r="C48" t="s">
-        <v>364</v>
-      </c>
       <c r="D48" t="s">
         <v>226</v>
       </c>
@@ -2740,17 +2909,17 @@
       <c r="F48" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J48" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>229</v>
       </c>
       <c r="B49" t="s">
         <v>230</v>
       </c>
-      <c r="C49" t="s">
-        <v>365</v>
-      </c>
       <c r="D49" t="s">
         <v>231</v>
       </c>
@@ -2760,17 +2929,17 @@
       <c r="F49" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J49" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>234</v>
       </c>
       <c r="B50" t="s">
         <v>235</v>
       </c>
-      <c r="C50" t="s">
-        <v>366</v>
-      </c>
       <c r="D50" t="s">
         <v>236</v>
       </c>
@@ -2780,17 +2949,17 @@
       <c r="F50" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J50" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>57</v>
       </c>
       <c r="B51" t="s">
         <v>239</v>
       </c>
-      <c r="C51" t="s">
-        <v>367</v>
-      </c>
       <c r="D51" t="s">
         <v>240</v>
       </c>
@@ -2799,6 +2968,9 @@
       </c>
       <c r="F51" t="s">
         <v>242</v>
+      </c>
+      <c r="J51" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>